<commit_message>
Added Raff's Alpha 1 Trace Matrix
</commit_message>
<xml_diff>
--- a/Documentation/Trace Matrices/Raffaele - Trace Matrix.xlsx
+++ b/Documentation/Trace Matrices/Raffaele - Trace Matrix.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21417"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GAME\Mccue David\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamb0057\Desktop\New folder\TeamTeam\Documentation\Trace Matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28CC9F9F-FAD6-4485-842E-8AE93BEAC763}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>Feature/User Story</t>
   </si>
@@ -109,13 +108,55 @@
   </si>
   <si>
     <t>406-550</t>
+  </si>
+  <si>
+    <t>Raffaele</t>
+  </si>
+  <si>
+    <t>Short/long wall 2-4,  floor 2-5</t>
+  </si>
+  <si>
+    <t>not really</t>
+  </si>
+  <si>
+    <t>Blueprinted rooms 2-6</t>
+  </si>
+  <si>
+    <t>All assets except the atomic one</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Particle system for loot</t>
+  </si>
+  <si>
+    <t>Partcile system for torch</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Bluprinted all assets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raffaele </t>
+  </si>
+  <si>
+    <t>UI design</t>
+  </si>
+  <si>
+    <t>GDD Asset section, Game Shell and Play screen as well as tweaking every other section</t>
+  </si>
+  <si>
+    <t>in google drive, not in code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,14 +642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
@@ -621,7 +662,7 @@
     <col min="9" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.45">
+    <row r="1" spans="1:8" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -645,7 +686,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -667,7 +708,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -688,7 +729,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
@@ -709,7 +750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -730,7 +771,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
@@ -751,79 +792,143 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="G7" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="G8" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="G9" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="G10" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="G11" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="G12" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="G13" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="G14" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -832,7 +937,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -841,7 +946,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -850,7 +955,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -859,7 +964,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -868,7 +973,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -877,9 +982,6 @@
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:7" ht="15"/>
-    <row r="22" spans="1:7" ht="15"/>
-    <row r="23" spans="1:7" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>